<commit_message>
updating latest lsoa analysis and outlier removal/cleaning.
</commit_message>
<xml_diff>
--- a/plots/toby-initial-lsoa-tests/mode-by-region-by-year.xlsx
+++ b/plots/toby-initial-lsoa-tests/mode-by-region-by-year.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toby.bridgeman\foe-work-on-cdrive\TransportBlackspots\plots\toby-initial-lsoa-tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3CF6C547-26B3-4EDF-89B7-5546466E9AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DC1D1A-0E15-436C-953E-9B971479A38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mode-by-region-by-year" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'mode-by-region-by-year'!$A$4:$U$60</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -59,9 +62,6 @@
   </si>
   <si>
     <t>Yorkshire and The Humber</t>
-  </si>
-  <si>
-    <t>tram</t>
   </si>
   <si>
     <t>metro</t>
@@ -120,11 +120,14 @@
   <si>
     <t>big drop off in rail 2018 onwards</t>
   </si>
+  <si>
+    <t>tram/light rail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -791,11 +794,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -809,21 +812,19 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="33" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="33" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="33" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -870,14 +871,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC1C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1206,31 +1200,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7">
         <v>2004</v>
@@ -1298,8 +1292,8 @@
       <c r="U4" s="8">
         <v>2023</v>
       </c>
-      <c r="V4" s="23" t="s">
-        <v>24</v>
+      <c r="V4" s="22" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1310,23 +1304,23 @@
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="19">
+        <v>32</v>
+      </c>
+      <c r="D5" s="18">
         <v>0.48139766296790598</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>0.495969189174087</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4">
         <v>0.96536898414110694</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="18">
         <v>0.56109402502949801</v>
       </c>
       <c r="M5" s="4">
@@ -1356,8 +1350,8 @@
       <c r="U5" s="5">
         <v>0.72784880859505097</v>
       </c>
-      <c r="V5" s="27" t="s">
-        <v>25</v>
+      <c r="V5" s="20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1368,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1390,7 +1384,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="5"/>
-      <c r="V6" s="21"/>
+      <c r="V6" s="20"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1400,7 +1394,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -1448,7 +1442,7 @@
       <c r="U7" s="5">
         <v>0.16910431831096101</v>
       </c>
-      <c r="V7" s="21"/>
+      <c r="V7" s="20"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1458,9 +1452,9 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="19">
+        <v>15</v>
+      </c>
+      <c r="D8" s="18">
         <v>0.57643123879638802</v>
       </c>
       <c r="E8" s="4">
@@ -1514,7 +1508,7 @@
       <c r="U8" s="5">
         <v>0.387605859554154</v>
       </c>
-      <c r="V8" s="21"/>
+      <c r="V8" s="20"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1524,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1544,7 +1538,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="5"/>
-      <c r="V9" s="21"/>
+      <c r="V9" s="20"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1554,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -1574,7 +1568,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
       <c r="U10" s="12"/>
-      <c r="V10" s="25"/>
+      <c r="V10" s="23"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1584,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1598,26 +1592,26 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="19">
+      <c r="P11" s="18">
         <v>0.348356890188812</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="Q11" s="18">
         <v>0.81677909131280302</v>
       </c>
-      <c r="R11" s="19">
+      <c r="R11" s="18">
         <v>6.8509486547325499E-2</v>
       </c>
-      <c r="S11" s="19">
-        <v>1</v>
-      </c>
-      <c r="T11" s="19">
+      <c r="S11" s="18">
+        <v>1</v>
+      </c>
+      <c r="T11" s="18">
         <v>0.61497940370273996</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="17">
         <v>0.35835260248380602</v>
       </c>
-      <c r="V11" s="24" t="s">
-        <v>23</v>
+      <c r="V11" s="27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1628,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1658,25 +1652,25 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="19">
+      <c r="P12" s="18">
         <v>0.313052275384195</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="18">
         <v>0.29585825661231002</v>
       </c>
-      <c r="R12" s="19">
+      <c r="R12" s="18">
         <v>0.35725942483774698</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="18">
         <v>0.28366593848015897</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="18">
         <v>0.28762264918916502</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="17">
         <v>0.28064630973993698</v>
       </c>
-      <c r="V12" s="24"/>
+      <c r="V12" s="27"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1686,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="4">
         <v>0.788608483942421</v>
@@ -1742,7 +1736,7 @@
       <c r="U13" s="5">
         <v>0.44843410891998597</v>
       </c>
-      <c r="V13" s="21"/>
+      <c r="V13" s="20"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -1752,7 +1746,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="15">
         <v>0.477802859292701</v>
@@ -1804,7 +1798,7 @@
       <c r="U14" s="16">
         <v>0.40124153498871301</v>
       </c>
-      <c r="V14" s="26"/>
+      <c r="V14" s="24"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -1814,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -1846,7 +1840,7 @@
       <c r="U15" s="12">
         <v>0.90325292006833602</v>
       </c>
-      <c r="V15" s="25"/>
+      <c r="V15" s="23"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1856,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1870,7 +1864,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <v>0.63405504447104999</v>
       </c>
       <c r="Q16" s="4">
@@ -1882,13 +1876,13 @@
       <c r="S16" s="4">
         <v>1</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="18">
         <v>0.81408493798573101</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="17">
         <v>0.61930693694055805</v>
       </c>
-      <c r="V16" s="21"/>
+      <c r="V16" s="20"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1898,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4">
         <v>0.97080536301354503</v>
@@ -1946,7 +1940,7 @@
       <c r="U17" s="5">
         <v>0.72403576205929598</v>
       </c>
-      <c r="V17" s="21"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1956,15 +1950,15 @@
         <v>3</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="19">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18">
         <v>4.0476676631402801E-2</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="18">
         <v>5.5711869198082499E-2</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="18">
         <v>0.104149305223793</v>
       </c>
       <c r="G18" s="4">
@@ -2012,7 +2006,7 @@
       <c r="U18" s="5">
         <v>0.83414095518452502</v>
       </c>
-      <c r="V18" s="21"/>
+      <c r="V18" s="20"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2022,7 +2016,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -2054,7 +2048,7 @@
       <c r="U19" s="16">
         <v>0.69958347140717903</v>
       </c>
-      <c r="V19" s="26"/>
+      <c r="V19" s="24"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2063,8 +2057,8 @@
       <c r="B20" s="3">
         <v>0</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>13</v>
+      <c r="C20" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2084,7 +2078,7 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="5"/>
-      <c r="V20" s="25"/>
+      <c r="V20" s="23"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2094,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2125,17 +2119,17 @@
       <c r="R21" s="4">
         <v>0.206988105471618</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="18">
         <v>0.12595894241470201</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="18">
         <v>5.6887069785790903E-2</v>
       </c>
-      <c r="U21" s="18">
+      <c r="U21" s="17">
         <v>2.6365662884879799E-2</v>
       </c>
-      <c r="V21" s="24" t="s">
-        <v>27</v>
+      <c r="V21" s="27" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -2146,7 +2140,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -2172,10 +2166,10 @@
       <c r="K22" s="4">
         <v>0.699850991676087</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
       <c r="P22" s="4">
         <v>0.30686998106199598</v>
       </c>
@@ -2185,16 +2179,16 @@
       <c r="R22" s="4">
         <v>0.26306024927697902</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="18">
         <v>0.30170882452251302</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="18">
         <v>0.29994714975703601</v>
       </c>
-      <c r="U22" s="18">
+      <c r="U22" s="17">
         <v>0.34233561372344601</v>
       </c>
-      <c r="V22" s="24"/>
+      <c r="V22" s="27"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -2204,9 +2198,9 @@
         <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="19">
+        <v>15</v>
+      </c>
+      <c r="D23" s="18">
         <v>2.4987390868857898E-4</v>
       </c>
       <c r="E23" s="4">
@@ -2251,17 +2245,17 @@
       <c r="R23" s="4">
         <v>0.11677319902536699</v>
       </c>
-      <c r="S23" s="19">
+      <c r="S23" s="18">
         <v>0.23847322957143199</v>
       </c>
-      <c r="T23" s="19">
+      <c r="T23" s="18">
         <v>0.234195182246343</v>
       </c>
-      <c r="U23" s="18">
+      <c r="U23" s="17">
         <v>0.21263811438435501</v>
       </c>
-      <c r="V23" s="21" t="s">
-        <v>26</v>
+      <c r="V23" s="20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -2272,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -2312,7 +2306,7 @@
       <c r="U24" s="16">
         <v>2.9673590504451001E-2</v>
       </c>
-      <c r="V24" s="26"/>
+      <c r="V24" s="24"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -2321,8 +2315,8 @@
       <c r="B25" s="3">
         <v>0</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>13</v>
+      <c r="C25" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -2338,10 +2332,10 @@
       <c r="M25" s="4">
         <v>0.64674627841265198</v>
       </c>
-      <c r="N25" s="19">
+      <c r="N25" s="18">
         <v>2.0138270805800499E-2</v>
       </c>
-      <c r="O25" s="19">
+      <c r="O25" s="18">
         <v>1.8405787214419201E-2</v>
       </c>
       <c r="P25" s="4">
@@ -2362,7 +2356,7 @@
       <c r="U25" s="5">
         <v>0.94520200938481502</v>
       </c>
-      <c r="V25" s="25"/>
+      <c r="V25" s="23"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -2372,12 +2366,12 @@
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="19">
+        <v>13</v>
+      </c>
+      <c r="D26" s="18">
         <v>0.69545528436404203</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="18">
         <v>1</v>
       </c>
       <c r="F26" s="4"/>
@@ -2396,8 +2390,8 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="5"/>
-      <c r="V26" s="21" t="s">
-        <v>29</v>
+      <c r="V26" s="20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
@@ -2408,12 +2402,12 @@
         <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="19">
-        <v>1</v>
-      </c>
-      <c r="E27" s="19">
+        <v>14</v>
+      </c>
+      <c r="D27" s="18">
+        <v>1</v>
+      </c>
+      <c r="E27" s="18">
         <v>0.73256709549797305</v>
       </c>
       <c r="F27" s="4">
@@ -2434,10 +2428,10 @@
       <c r="K27" s="4">
         <v>0.75477542473940396</v>
       </c>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
       <c r="P27" s="4">
         <v>0.31850913312476298</v>
       </c>
@@ -2456,7 +2450,7 @@
       <c r="U27" s="5">
         <v>0.34496415494044502</v>
       </c>
-      <c r="V27" s="21"/>
+      <c r="V27" s="20"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -2466,9 +2460,9 @@
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="19">
+        <v>15</v>
+      </c>
+      <c r="D28" s="18">
         <v>0.41712815162891198</v>
       </c>
       <c r="E28" s="4">
@@ -2522,7 +2516,7 @@
       <c r="U28" s="5">
         <v>0.53648323654915897</v>
       </c>
-      <c r="V28" s="21"/>
+      <c r="V28" s="20"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -2532,7 +2526,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4">
@@ -2574,7 +2568,7 @@
       <c r="U29" s="5">
         <v>0.33826138379657</v>
       </c>
-      <c r="V29" s="26"/>
+      <c r="V29" s="24"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -2583,8 +2577,8 @@
       <c r="B30" s="10">
         <v>0</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>13</v>
+      <c r="C30" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -2624,7 +2618,7 @@
       <c r="U30" s="12">
         <v>0.92596406215382698</v>
       </c>
-      <c r="V30" s="25"/>
+      <c r="V30" s="23"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -2634,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2654,7 +2648,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="5"/>
-      <c r="V31" s="21"/>
+      <c r="V31" s="20"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -2664,7 +2658,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="4">
         <v>1</v>
@@ -2712,7 +2706,7 @@
       <c r="U32" s="5">
         <v>0.25040892381913699</v>
       </c>
-      <c r="V32" s="21"/>
+      <c r="V32" s="20"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2722,9 +2716,9 @@
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="19">
+        <v>15</v>
+      </c>
+      <c r="D33" s="18">
         <v>0.168302598366627</v>
       </c>
       <c r="E33" s="4">
@@ -2778,7 +2772,7 @@
       <c r="U33" s="5">
         <v>0.26134928606541602</v>
       </c>
-      <c r="V33" s="21"/>
+      <c r="V33" s="20"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
@@ -2788,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -2828,7 +2822,7 @@
       <c r="U34" s="16">
         <v>1</v>
       </c>
-      <c r="V34" s="26"/>
+      <c r="V34" s="24"/>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -2837,8 +2831,8 @@
       <c r="B35" s="3">
         <v>0</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>13</v>
+      <c r="C35" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2872,7 +2866,7 @@
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="5"/>
-      <c r="V35" s="25"/>
+      <c r="V35" s="23"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -2882,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2918,7 +2912,7 @@
       <c r="U36" s="5">
         <v>0.61674623182964095</v>
       </c>
-      <c r="V36" s="21"/>
+      <c r="V36" s="20"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2928,7 +2922,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="4">
         <v>0.96497954680630005</v>
@@ -2976,7 +2970,7 @@
       <c r="U37" s="5">
         <v>0.28449477745574597</v>
       </c>
-      <c r="V37" s="21"/>
+      <c r="V37" s="20"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -2986,7 +2980,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="4">
         <v>0.79385619887376502</v>
@@ -3042,7 +3036,7 @@
       <c r="U38" s="5">
         <v>0.51752971815022497</v>
       </c>
-      <c r="V38" s="21"/>
+      <c r="V38" s="20"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -3052,7 +3046,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39" s="4">
         <v>0.84606975424138597</v>
@@ -3108,7 +3102,7 @@
       <c r="U39" s="5">
         <v>0.67127420270355498</v>
       </c>
-      <c r="V39" s="26"/>
+      <c r="V39" s="24"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
@@ -3118,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -3138,7 +3132,7 @@
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
       <c r="U40" s="12"/>
-      <c r="V40" s="25"/>
+      <c r="V40" s="23"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -3148,7 +3142,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -3168,7 +3162,7 @@
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
       <c r="U41" s="5"/>
-      <c r="V41" s="21"/>
+      <c r="V41" s="20"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -3178,7 +3172,7 @@
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -3205,9 +3199,9 @@
         <v>0.74696209093452604</v>
       </c>
       <c r="L42" s="4"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
       <c r="P42" s="4">
         <v>0.145077606383644</v>
       </c>
@@ -3226,7 +3220,7 @@
       <c r="U42" s="5">
         <v>0.187134954344789</v>
       </c>
-      <c r="V42" s="21"/>
+      <c r="V42" s="20"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -3236,7 +3230,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="4">
         <v>0.814363546242868</v>
@@ -3292,7 +3286,7 @@
       <c r="U43" s="5">
         <v>0.46866417270059402</v>
       </c>
-      <c r="V43" s="21"/>
+      <c r="V43" s="20"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
@@ -3302,7 +3296,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -3342,7 +3336,7 @@
       <c r="U44" s="16">
         <v>0.78978853491977996</v>
       </c>
-      <c r="V44" s="26"/>
+      <c r="V44" s="24"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -3351,8 +3345,8 @@
       <c r="B45" s="3">
         <v>0</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>13</v>
+      <c r="C45" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -3372,7 +3366,7 @@
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
       <c r="U45" s="5"/>
-      <c r="V45" s="25"/>
+      <c r="V45" s="23"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -3382,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -3402,7 +3396,7 @@
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
       <c r="U46" s="5"/>
-      <c r="V46" s="21"/>
+      <c r="V46" s="20"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -3412,7 +3406,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -3442,26 +3436,26 @@
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
-      <c r="P47" s="19">
+      <c r="P47" s="18">
         <v>0.16116059003295699</v>
       </c>
-      <c r="Q47" s="19">
+      <c r="Q47" s="18">
         <v>0.14746675670746401</v>
       </c>
-      <c r="R47" s="19">
+      <c r="R47" s="18">
         <v>0.153008715247756</v>
       </c>
-      <c r="S47" s="19">
+      <c r="S47" s="18">
         <v>0.144191499533844</v>
       </c>
-      <c r="T47" s="19">
+      <c r="T47" s="18">
         <v>0.16076894037446801</v>
       </c>
-      <c r="U47" s="18">
+      <c r="U47" s="17">
         <v>0.143189896087698</v>
       </c>
-      <c r="V47" s="21" t="s">
-        <v>32</v>
+      <c r="V47" s="20" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
@@ -3472,7 +3466,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48" s="4">
         <v>0.81924161889343505</v>
@@ -3528,7 +3522,7 @@
       <c r="U48" s="5">
         <v>0.42131636965150598</v>
       </c>
-      <c r="V48" s="21"/>
+      <c r="V48" s="20"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -3538,7 +3532,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -3552,26 +3546,26 @@
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
-      <c r="P49" s="19">
+      <c r="P49" s="18">
         <v>0.32038834951456302</v>
       </c>
-      <c r="Q49" s="19">
+      <c r="Q49" s="18">
         <v>0.87378640776699001</v>
       </c>
-      <c r="R49" s="19">
+      <c r="R49" s="18">
         <v>0.87378640776699001</v>
       </c>
-      <c r="S49" s="19">
+      <c r="S49" s="18">
         <v>0.92233009708737901</v>
       </c>
-      <c r="T49" s="19">
+      <c r="T49" s="18">
         <v>0.91262135922330101</v>
       </c>
-      <c r="U49" s="18">
-        <v>1</v>
-      </c>
-      <c r="V49" s="26" t="s">
-        <v>28</v>
+      <c r="U49" s="17">
+        <v>1</v>
+      </c>
+      <c r="V49" s="24" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
@@ -3590,7 +3584,7 @@
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
-      <c r="L50" s="28">
+      <c r="L50" s="25">
         <v>1</v>
       </c>
       <c r="M50" s="15"/>
@@ -3602,8 +3596,8 @@
       <c r="S50" s="15"/>
       <c r="T50" s="15"/>
       <c r="U50" s="16"/>
-      <c r="V50" s="21" t="s">
-        <v>30</v>
+      <c r="V50" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -3614,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
@@ -3654,7 +3648,7 @@
       <c r="U51" s="12">
         <v>0.54910182493924797</v>
       </c>
-      <c r="V51" s="25"/>
+      <c r="V51" s="23"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -3664,7 +3658,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4">
@@ -3686,7 +3680,7 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="5"/>
-      <c r="V52" s="21"/>
+      <c r="V52" s="20"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
@@ -3696,7 +3690,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -3726,26 +3720,26 @@
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
-      <c r="P53" s="19">
+      <c r="P53" s="18">
         <v>0.22706176046194901</v>
       </c>
-      <c r="Q53" s="19">
+      <c r="Q53" s="18">
         <v>0.21566903694141801</v>
       </c>
-      <c r="R53" s="19">
+      <c r="R53" s="18">
         <v>0.20399178444398899</v>
       </c>
-      <c r="S53" s="19">
+      <c r="S53" s="18">
         <v>0.182383510585722</v>
       </c>
-      <c r="T53" s="19">
+      <c r="T53" s="18">
         <v>0.18463879548236101</v>
       </c>
-      <c r="U53" s="18">
+      <c r="U53" s="17">
         <v>0.20748184654942101</v>
       </c>
-      <c r="V53" s="21" t="s">
-        <v>31</v>
+      <c r="V53" s="20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -3756,9 +3750,9 @@
         <v>3</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="19">
+        <v>15</v>
+      </c>
+      <c r="D54" s="18">
         <v>0.60628102149408802</v>
       </c>
       <c r="E54" s="4">
@@ -3812,7 +3806,7 @@
       <c r="U54" s="5">
         <v>0.50345417235864498</v>
       </c>
-      <c r="V54" s="21"/>
+      <c r="V54" s="20"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
@@ -3822,7 +3816,7 @@
         <v>4</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -3842,7 +3836,7 @@
       <c r="S55" s="15"/>
       <c r="T55" s="15"/>
       <c r="U55" s="16"/>
-      <c r="V55" s="26"/>
+      <c r="V55" s="24"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
@@ -3852,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
@@ -3891,10 +3885,10 @@
       <c r="T56" s="11">
         <v>0.80068988812348396</v>
       </c>
-      <c r="U56" s="29">
+      <c r="U56" s="26">
         <v>1.7920714044443498E-2</v>
       </c>
-      <c r="V56" s="21"/>
+      <c r="V56" s="20"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
@@ -3904,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4">
@@ -3926,7 +3920,7 @@
       <c r="S57" s="4"/>
       <c r="T57" s="4"/>
       <c r="U57" s="5"/>
-      <c r="V57" s="21"/>
+      <c r="V57" s="20"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -3936,7 +3930,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -3984,8 +3978,8 @@
       <c r="U58" s="5">
         <v>0.29202003370148699</v>
       </c>
-      <c r="V58" s="21" t="s">
-        <v>31</v>
+      <c r="V58" s="20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
@@ -3996,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" s="4">
         <v>1</v>
@@ -4052,7 +4046,7 @@
       <c r="U59" s="5">
         <v>0.32890448106518999</v>
       </c>
-      <c r="V59" s="21"/>
+      <c r="V59" s="20"/>
     </row>
     <row r="60" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
@@ -4062,7 +4056,7 @@
         <v>4</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
@@ -4082,10 +4076,10 @@
       <c r="S60" s="15"/>
       <c r="T60" s="15"/>
       <c r="U60" s="16"/>
-      <c r="V60" s="22"/>
+      <c r="V60" s="21"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
+      <c r="A61" s="2"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -4106,7 +4100,7 @@
       <c r="U61" s="1"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
+      <c r="A62" s="2"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -4127,22 +4121,23 @@
       <c r="U62" s="1"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A4:U60" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="V11:V12"/>
     <mergeCell ref="V21:V22"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:U60 A63:A64">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+  <conditionalFormatting sqref="A63:A64 A4:U60">
+    <cfRule type="containsBlanks" dxfId="1" priority="4">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>